<commit_message>
one minor change to fix text in V-4442
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-windows-2012r2-member-server-stig-overlay_20181227.xlsx
+++ b/cms-ars-3.1-high-microsoft-windows-2012r2-member-server-stig-overlay_20181227.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-high-microsoft-windows-2012r2-member-server-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E9C15F2-DED5-4CC9-A097-7431BCDBCBAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5AE85F-BAB0-9345-B47B-93E466206F30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="8532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="W2012r2MS" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">W2012r2MS!$A$1:$AA$339</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -12027,54 +12028,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>5 (or less)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Configure the policy value for Computer Configuration -&gt; Windows Settings -&gt; Security Settings -&gt; Local Policies -&gt; Security Options -&gt; "MSS: (ScreenSaverGracePeriod) The time in seconds before the screen saver grace period expires (0 recommended)" to "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or less</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-(See "Updating the Windows Security Options File" in the STIG Overview document if MSS settings are not visible in the system's policy tools.)</t>
     </r>
   </si>
   <si>
@@ -14079,12 +14032,110 @@
   <si>
     <t>V-1121</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Configure the policy value for Computer Configuration -&gt; Windows Settings -&gt; Security Settings -&gt; Local Policies -&gt; Security Options -&gt; "MSS: (ScreenSaverGracePeriod) The time in seconds before the screen saver grace period expires </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve">must be </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>recommended)" to "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>" or less</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+(See "Updating the Windows Security Options File" in the STIG Overview document if MSS settings are not visible in the system's policy tools.)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14258,6 +14309,35 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="34">
@@ -15018,46 +15098,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA339"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B91" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="8" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="8" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="8" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="8" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" style="8" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="50.44140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="8" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="50.5" style="8" customWidth="1"/>
     <col min="10" max="10" width="37.6640625" style="8" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" style="8" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" style="8" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" style="8" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" style="8" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="14.77734375" style="8" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" style="8" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" style="8" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" style="8" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" style="8" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="16" style="8" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" style="8" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="8" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="145.33203125" style="8" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="22" style="8" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="11.77734375" style="8" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="11.83203125" style="8" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="119.6640625" style="8" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="16.109375" style="8" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="26.88671875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="16.109375" style="8" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" style="7"/>
+    <col min="23" max="23" width="16.1640625" style="8" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="26.83203125" style="8" customWidth="1"/>
+    <col min="25" max="25" width="16.1640625" style="8" customWidth="1"/>
+    <col min="26" max="26" width="8.83203125" style="7"/>
     <col min="27" max="27" width="11" style="7" hidden="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="8"/>
+    <col min="28" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -15137,7 +15217,7 @@
         <v>2673</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="176">
       <c r="A2" s="9" t="s">
         <v>2617</v>
       </c>
@@ -15197,7 +15277,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" ht="192">
       <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
@@ -15257,7 +15337,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" ht="192">
       <c r="A4" s="9" t="s">
         <v>2680</v>
       </c>
@@ -15317,7 +15397,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" ht="160">
       <c r="A5" s="9" t="s">
         <v>2681</v>
       </c>
@@ -15377,7 +15457,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" ht="240">
       <c r="A6" s="9" t="s">
         <v>2682</v>
       </c>
@@ -15437,7 +15517,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="256">
       <c r="A7" s="9" t="s">
         <v>2683</v>
       </c>
@@ -15497,7 +15577,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" ht="192">
       <c r="A8" s="9" t="s">
         <v>2679</v>
       </c>
@@ -15557,7 +15637,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="409.6">
       <c r="A9" s="6" t="s">
         <v>83</v>
       </c>
@@ -15617,7 +15697,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" ht="335">
       <c r="A10" s="9" t="s">
         <v>2684</v>
       </c>
@@ -15677,7 +15757,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" ht="160">
       <c r="A11" s="9" t="s">
         <v>97</v>
       </c>
@@ -15737,7 +15817,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" ht="272">
       <c r="A12" s="9" t="s">
         <v>2740</v>
       </c>
@@ -15797,7 +15877,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" ht="409.6">
       <c r="A13" s="6" t="s">
         <v>2745</v>
       </c>
@@ -15857,7 +15937,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" ht="272">
       <c r="A14" s="6" t="s">
         <v>2741</v>
       </c>
@@ -15917,7 +15997,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" ht="365">
       <c r="A15" s="9" t="s">
         <v>2685</v>
       </c>
@@ -15977,7 +16057,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" ht="176">
       <c r="A16" s="9" t="s">
         <v>131</v>
       </c>
@@ -16037,7 +16117,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" ht="176">
       <c r="A17" s="9" t="s">
         <v>140</v>
       </c>
@@ -16097,7 +16177,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" ht="304">
       <c r="A18" s="6" t="s">
         <v>149</v>
       </c>
@@ -16157,7 +16237,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" ht="409.6">
       <c r="A19" s="6" t="s">
         <v>2615</v>
       </c>
@@ -16217,7 +16297,7 @@
         <v>2629</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" ht="192">
       <c r="A20" s="2" t="s">
         <v>160</v>
       </c>
@@ -16277,9 +16357,9 @@
         <v>2630</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="208">
       <c r="A21" s="9" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>24</v>
@@ -16337,9 +16417,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" ht="144">
       <c r="A22" s="9" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>24</v>
@@ -16397,9 +16477,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" ht="176">
       <c r="A23" s="9" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>24</v>
@@ -16457,7 +16537,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" ht="409.6">
       <c r="A24" s="12" t="s">
         <v>2766</v>
       </c>
@@ -16517,9 +16597,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" ht="409.6">
       <c r="A25" s="9" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>45</v>
@@ -16577,7 +16657,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" ht="409.6">
       <c r="A26" s="9" t="s">
         <v>2686</v>
       </c>
@@ -16637,9 +16717,9 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" ht="208">
       <c r="A27" s="9" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>60</v>
@@ -16697,9 +16777,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" ht="288">
       <c r="A28" s="9" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>60</v>
@@ -16757,7 +16837,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" ht="350">
       <c r="A29" s="9" t="s">
         <v>225</v>
       </c>
@@ -16817,7 +16897,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" ht="240">
       <c r="A30" s="9" t="s">
         <v>234</v>
       </c>
@@ -16877,7 +16957,7 @@
         <v>2632</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" ht="304">
       <c r="A31" s="9" t="s">
         <v>243</v>
       </c>
@@ -16939,7 +17019,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" ht="409.6">
       <c r="A32" s="9" t="s">
         <v>252</v>
       </c>
@@ -16999,7 +17079,7 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" ht="192">
       <c r="A33" s="6" t="s">
         <v>261</v>
       </c>
@@ -17055,13 +17135,13 @@
         <v>269</v>
       </c>
       <c r="Y33" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA33" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" ht="335">
       <c r="A34" s="9" t="s">
         <v>2687</v>
       </c>
@@ -17121,7 +17201,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" ht="288">
       <c r="A35" s="9" t="s">
         <v>277</v>
       </c>
@@ -17181,7 +17261,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" ht="304">
       <c r="A36" s="9" t="s">
         <v>285</v>
       </c>
@@ -17241,9 +17321,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" ht="409.6">
       <c r="A37" s="9" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>24</v>
@@ -17301,7 +17381,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" ht="288">
       <c r="A38" s="9" t="s">
         <v>300</v>
       </c>
@@ -17361,7 +17441,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" ht="350">
       <c r="A39" s="9" t="s">
         <v>308</v>
       </c>
@@ -17421,7 +17501,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" ht="350">
       <c r="A40" s="9" t="s">
         <v>317</v>
       </c>
@@ -17481,7 +17561,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" ht="350">
       <c r="A41" s="9" t="s">
         <v>325</v>
       </c>
@@ -17541,7 +17621,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" ht="224">
       <c r="A42" s="9" t="s">
         <v>333</v>
       </c>
@@ -17601,7 +17681,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" ht="350">
       <c r="A43" s="9" t="s">
         <v>341</v>
       </c>
@@ -17661,7 +17741,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" ht="224">
       <c r="A44" s="9" t="s">
         <v>349</v>
       </c>
@@ -17721,7 +17801,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" ht="176">
       <c r="A45" s="9" t="s">
         <v>357</v>
       </c>
@@ -17781,7 +17861,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" ht="208">
       <c r="A46" s="9" t="s">
         <v>365</v>
       </c>
@@ -17841,7 +17921,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" ht="272">
       <c r="A47" s="9" t="s">
         <v>373</v>
       </c>
@@ -17901,7 +17981,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" ht="365">
       <c r="A48" s="1" t="s">
         <v>2760</v>
       </c>
@@ -17961,7 +18041,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" ht="176">
       <c r="A49" s="9" t="s">
         <v>387</v>
       </c>
@@ -18021,7 +18101,7 @@
         <v>2632</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" ht="272">
       <c r="A50" s="9" t="s">
         <v>396</v>
       </c>
@@ -18081,7 +18161,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" ht="144">
       <c r="A51" s="9" t="s">
         <v>405</v>
       </c>
@@ -18143,7 +18223,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" ht="350">
       <c r="A52" s="2" t="s">
         <v>414</v>
       </c>
@@ -18203,7 +18283,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" ht="208">
       <c r="A53" s="9" t="s">
         <v>422</v>
       </c>
@@ -18265,7 +18345,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" ht="144">
       <c r="A54" s="9" t="s">
         <v>431</v>
       </c>
@@ -18325,7 +18405,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" ht="288">
       <c r="A55" s="2" t="s">
         <v>439</v>
       </c>
@@ -18385,7 +18465,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" ht="350">
       <c r="A56" s="2" t="s">
         <v>447</v>
       </c>
@@ -18445,7 +18525,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" ht="224">
       <c r="A57" s="2" t="s">
         <v>455</v>
       </c>
@@ -18505,7 +18585,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" ht="176">
       <c r="A58" s="2" t="s">
         <v>463</v>
       </c>
@@ -18565,7 +18645,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" ht="256">
       <c r="A59" s="9" t="s">
         <v>471</v>
       </c>
@@ -18625,7 +18705,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="60" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" ht="192">
       <c r="A60" s="6" t="s">
         <v>479</v>
       </c>
@@ -18685,7 +18765,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" ht="350">
       <c r="A61" s="9" t="s">
         <v>484</v>
       </c>
@@ -18745,7 +18825,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" ht="160">
       <c r="A62" s="6" t="s">
         <v>492</v>
       </c>
@@ -18801,13 +18881,13 @@
         <v>500</v>
       </c>
       <c r="Y62" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA62" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" ht="160">
       <c r="A63" s="9" t="s">
         <v>501</v>
       </c>
@@ -18867,7 +18947,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" ht="160">
       <c r="A64" s="9" t="s">
         <v>509</v>
       </c>
@@ -18927,7 +19007,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:27" ht="176">
       <c r="A65" s="9" t="s">
         <v>517</v>
       </c>
@@ -18987,7 +19067,7 @@
         <v>2632</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:27" ht="224">
       <c r="A66" s="9" t="s">
         <v>525</v>
       </c>
@@ -19047,7 +19127,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:27" ht="160">
       <c r="A67" s="9" t="s">
         <v>533</v>
       </c>
@@ -19107,7 +19187,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:27" ht="176">
       <c r="A68" s="9" t="s">
         <v>541</v>
       </c>
@@ -19167,7 +19247,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:27" ht="272">
       <c r="A69" s="2" t="s">
         <v>549</v>
       </c>
@@ -19227,7 +19307,7 @@
         <v>2638</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:27" ht="192">
       <c r="A70" s="9" t="s">
         <v>558</v>
       </c>
@@ -19287,7 +19367,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="71" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:27" ht="208">
       <c r="A71" s="9" t="s">
         <v>566</v>
       </c>
@@ -19349,7 +19429,7 @@
         <v>2639</v>
       </c>
     </row>
-    <row r="72" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:27" ht="176">
       <c r="A72" s="6" t="s">
         <v>576</v>
       </c>
@@ -19405,13 +19485,13 @@
         <v>500</v>
       </c>
       <c r="Y72" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA72" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="73" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:27" ht="350">
       <c r="A73" s="9" t="s">
         <v>2677</v>
       </c>
@@ -19471,7 +19551,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" ht="192">
       <c r="A74" s="9" t="s">
         <v>592</v>
       </c>
@@ -19531,7 +19611,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:27" ht="176">
       <c r="A75" s="9" t="s">
         <v>600</v>
       </c>
@@ -19591,7 +19671,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:27" ht="256">
       <c r="A76" s="9" t="s">
         <v>608</v>
       </c>
@@ -19651,7 +19731,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="77" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:27" ht="176">
       <c r="A77" s="2" t="s">
         <v>616</v>
       </c>
@@ -19711,9 +19791,9 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="78" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:27" ht="409.6">
       <c r="A78" s="2" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>60</v>
@@ -19728,17 +19808,17 @@
         <v>626</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>627</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4" t="s">
+        <v>2817</v>
+      </c>
+      <c r="J78" s="4" t="s">
         <v>2818</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>2819</v>
       </c>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
@@ -19771,7 +19851,7 @@
         <v>2641</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:27" ht="335">
       <c r="A79" s="9" t="s">
         <v>629</v>
       </c>
@@ -19831,7 +19911,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="80" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:27" ht="224">
       <c r="A80" s="6" t="s">
         <v>637</v>
       </c>
@@ -19887,13 +19967,13 @@
         <v>269</v>
       </c>
       <c r="Y80" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA80" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:27" ht="288">
       <c r="A81" s="6" t="s">
         <v>645</v>
       </c>
@@ -19949,13 +20029,13 @@
         <v>269</v>
       </c>
       <c r="Y81" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA81" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:27" ht="409.6">
       <c r="A82" s="2" t="s">
         <v>653</v>
       </c>
@@ -20015,7 +20095,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="83" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:27" ht="176">
       <c r="A83" s="9" t="s">
         <v>662</v>
       </c>
@@ -20075,7 +20155,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:27" ht="409.6">
       <c r="A84" s="6" t="s">
         <v>669</v>
       </c>
@@ -20135,7 +20215,7 @@
         <v>2643</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:27" ht="192">
       <c r="A85" s="9" t="s">
         <v>676</v>
       </c>
@@ -20195,7 +20275,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:27" ht="176">
       <c r="A86" s="9" t="s">
         <v>684</v>
       </c>
@@ -20255,7 +20335,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="87" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:27" ht="176">
       <c r="A87" s="2" t="s">
         <v>692</v>
       </c>
@@ -20315,7 +20395,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:27" ht="176">
       <c r="A88" s="2" t="s">
         <v>701</v>
       </c>
@@ -20375,7 +20455,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:27" ht="224">
       <c r="A89" s="2" t="s">
         <v>709</v>
       </c>
@@ -20435,7 +20515,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:27" ht="176">
       <c r="A90" s="2" t="s">
         <v>717</v>
       </c>
@@ -20495,7 +20575,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:27" ht="192">
       <c r="A91" s="1" t="s">
         <v>2767</v>
       </c>
@@ -20522,7 +20602,7 @@
         <v>2768</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>2769</v>
+        <v>2850</v>
       </c>
       <c r="K91" s="5"/>
       <c r="L91" s="5"/>
@@ -20555,7 +20635,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="92" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:27" ht="409.6">
       <c r="A92" s="2" t="s">
         <v>730</v>
       </c>
@@ -20615,7 +20695,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="93" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:27" ht="409.6">
       <c r="A93" s="2" t="s">
         <v>738</v>
       </c>
@@ -20679,9 +20759,9 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="94" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:27" ht="288">
       <c r="A94" s="9" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>24</v>
@@ -20739,7 +20819,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="95" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:27" ht="208">
       <c r="A95" s="9" t="s">
         <v>2688</v>
       </c>
@@ -20799,7 +20879,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="96" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:27" ht="350">
       <c r="A96" s="9" t="s">
         <v>763</v>
       </c>
@@ -20859,7 +20939,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="97" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:27" ht="350">
       <c r="A97" s="9" t="s">
         <v>771</v>
       </c>
@@ -20919,7 +20999,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:27" ht="350">
       <c r="A98" s="9" t="s">
         <v>779</v>
       </c>
@@ -20979,7 +21059,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="99" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:27" ht="240">
       <c r="A99" s="2" t="s">
         <v>787</v>
       </c>
@@ -21039,7 +21119,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="100" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:27" ht="192">
       <c r="A100" s="6" t="s">
         <v>795</v>
       </c>
@@ -21099,7 +21179,7 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="101" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:27" ht="409.6">
       <c r="A101" s="9" t="s">
         <v>801</v>
       </c>
@@ -21159,7 +21239,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="102" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:27" ht="395">
       <c r="A102" s="9" t="s">
         <v>809</v>
       </c>
@@ -21219,7 +21299,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="103" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:27" ht="192">
       <c r="A103" s="9" t="s">
         <v>817</v>
       </c>
@@ -21279,9 +21359,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="104" spans="1:27" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:27" ht="409.6">
       <c r="A104" s="1" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>24</v>
@@ -21296,17 +21376,17 @@
         <v>827</v>
       </c>
       <c r="F104" s="4" t="s">
+        <v>2771</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>2772</v>
-      </c>
-      <c r="G104" s="4" t="s">
-        <v>2773</v>
       </c>
       <c r="H104" s="5"/>
       <c r="I104" s="4" t="s">
+        <v>2769</v>
+      </c>
+      <c r="J104" s="4" t="s">
         <v>2770</v>
-      </c>
-      <c r="J104" s="4" t="s">
-        <v>2771</v>
       </c>
       <c r="K104" s="5"/>
       <c r="L104" s="5"/>
@@ -21339,7 +21419,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="105" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:27" ht="409.6">
       <c r="A105" s="6" t="s">
         <v>828</v>
       </c>
@@ -21395,13 +21475,13 @@
         <v>836</v>
       </c>
       <c r="Y105" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA105" s="10" t="s">
         <v>2645</v>
       </c>
     </row>
-    <row r="106" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:27" ht="409.6">
       <c r="A106" s="6" t="s">
         <v>837</v>
       </c>
@@ -21457,15 +21537,15 @@
         <v>836</v>
       </c>
       <c r="Y106" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA106" s="10" t="s">
         <v>2645</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:27" ht="350">
       <c r="A107" s="9" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>24</v>
@@ -21523,7 +21603,7 @@
         <v>2646</v>
       </c>
     </row>
-    <row r="108" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:27" ht="192">
       <c r="A108" s="9" t="s">
         <v>853</v>
       </c>
@@ -21583,7 +21663,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="109" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:27" ht="224">
       <c r="A109" s="6" t="s">
         <v>861</v>
       </c>
@@ -21639,13 +21719,13 @@
         <v>500</v>
       </c>
       <c r="Y109" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA109" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="110" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:27" ht="272">
       <c r="A110" s="2" t="s">
         <v>869</v>
       </c>
@@ -21705,7 +21785,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="111" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:27" ht="224">
       <c r="A111" s="6" t="s">
         <v>878</v>
       </c>
@@ -21761,13 +21841,13 @@
         <v>500</v>
       </c>
       <c r="Y111" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA111" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="112" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:27" ht="224">
       <c r="A112" s="2" t="s">
         <v>886</v>
       </c>
@@ -21827,7 +21907,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="113" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:27" ht="240">
       <c r="A113" s="2" t="s">
         <v>894</v>
       </c>
@@ -21887,7 +21967,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="114" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:27" ht="224">
       <c r="A114" s="6" t="s">
         <v>902</v>
       </c>
@@ -21943,13 +22023,13 @@
         <v>500</v>
       </c>
       <c r="Y114" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA114" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="115" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:27" ht="224">
       <c r="A115" s="2" t="s">
         <v>910</v>
       </c>
@@ -22009,7 +22089,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="116" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:27" ht="224">
       <c r="A116" s="2" t="s">
         <v>918</v>
       </c>
@@ -22069,7 +22149,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="117" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:27" ht="192">
       <c r="A117" s="2" t="s">
         <v>926</v>
       </c>
@@ -22129,7 +22209,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="118" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:27" ht="176">
       <c r="A118" s="6" t="s">
         <v>934</v>
       </c>
@@ -22185,13 +22265,13 @@
         <v>500</v>
       </c>
       <c r="Y118" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA118" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="119" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:27" ht="176">
       <c r="A119" s="2" t="s">
         <v>942</v>
       </c>
@@ -22251,7 +22331,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="120" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:27" ht="208">
       <c r="A120" s="6" t="s">
         <v>950</v>
       </c>
@@ -22307,13 +22387,13 @@
         <v>958</v>
       </c>
       <c r="Y120" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA120" s="10" t="s">
         <v>2648</v>
       </c>
     </row>
-    <row r="121" spans="1:27" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:27" ht="320">
       <c r="A121" s="2" t="s">
         <v>959</v>
       </c>
@@ -22373,7 +22453,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="122" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:27" ht="272">
       <c r="A122" s="2" t="s">
         <v>967</v>
       </c>
@@ -22433,7 +22513,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="123" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:27" ht="304">
       <c r="A123" s="6" t="s">
         <v>975</v>
       </c>
@@ -22489,13 +22569,13 @@
         <v>269</v>
       </c>
       <c r="Y123" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA123" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="124" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:27" ht="192">
       <c r="A124" s="9" t="s">
         <v>983</v>
       </c>
@@ -22555,7 +22635,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="125" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:27" ht="192">
       <c r="A125" s="9" t="s">
         <v>991</v>
       </c>
@@ -22615,7 +22695,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="126" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:27" ht="192">
       <c r="A126" s="9" t="s">
         <v>999</v>
       </c>
@@ -22675,9 +22755,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="127" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:27" ht="176">
       <c r="A127" s="2" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>24</v>
@@ -22735,7 +22815,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="128" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:27" ht="160">
       <c r="A128" s="2" t="s">
         <v>1014</v>
       </c>
@@ -22795,7 +22875,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="129" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:27" ht="176">
       <c r="A129" s="2" t="s">
         <v>1022</v>
       </c>
@@ -22855,7 +22935,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="130" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:27" ht="160">
       <c r="A130" s="2" t="s">
         <v>1030</v>
       </c>
@@ -22915,7 +22995,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="131" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:27" ht="288">
       <c r="A131" s="2" t="s">
         <v>1038</v>
       </c>
@@ -22975,7 +23055,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="132" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:27" ht="224">
       <c r="A132" s="9" t="s">
         <v>1046</v>
       </c>
@@ -23035,7 +23115,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="133" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:27" ht="176">
       <c r="A133" s="9" t="s">
         <v>1054</v>
       </c>
@@ -23095,7 +23175,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="134" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:27" ht="192">
       <c r="A134" s="9" t="s">
         <v>1062</v>
       </c>
@@ -23155,7 +23235,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="135" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:27" ht="160">
       <c r="A135" s="9" t="s">
         <v>1070</v>
       </c>
@@ -23215,7 +23295,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="136" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:27" ht="176">
       <c r="A136" s="6" t="s">
         <v>1078</v>
       </c>
@@ -23271,13 +23351,13 @@
         <v>269</v>
       </c>
       <c r="Y136" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA136" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="137" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:27" ht="176">
       <c r="A137" s="6" t="s">
         <v>1086</v>
       </c>
@@ -23333,13 +23413,13 @@
         <v>269</v>
       </c>
       <c r="Y137" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA137" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="138" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:27" ht="335">
       <c r="A138" s="9" t="s">
         <v>1094</v>
       </c>
@@ -23399,7 +23479,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="139" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:27" ht="208">
       <c r="A139" s="2" t="s">
         <v>1102</v>
       </c>
@@ -23459,7 +23539,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="140" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:27" ht="208">
       <c r="A140" s="2" t="s">
         <v>1110</v>
       </c>
@@ -23519,7 +23599,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="141" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:27" ht="240">
       <c r="A141" s="2" t="s">
         <v>1118</v>
       </c>
@@ -23579,7 +23659,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="142" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:27" ht="192">
       <c r="A142" s="2" t="s">
         <v>1126</v>
       </c>
@@ -23639,7 +23719,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="143" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:27" ht="176">
       <c r="A143" s="2" t="s">
         <v>1134</v>
       </c>
@@ -23699,7 +23779,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="144" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:27" ht="176">
       <c r="A144" s="9" t="s">
         <v>1142</v>
       </c>
@@ -23759,7 +23839,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="145" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:27" ht="272">
       <c r="A145" s="2" t="s">
         <v>1150</v>
       </c>
@@ -23819,7 +23899,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="146" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:27" ht="272">
       <c r="A146" s="6" t="s">
         <v>1158</v>
       </c>
@@ -23875,13 +23955,13 @@
         <v>269</v>
       </c>
       <c r="Y146" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA146" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="147" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:27" ht="288">
       <c r="A147" s="2" t="s">
         <v>1166</v>
       </c>
@@ -23941,7 +24021,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="148" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:27" ht="192">
       <c r="A148" s="6" t="s">
         <v>1174</v>
       </c>
@@ -23997,13 +24077,13 @@
         <v>500</v>
       </c>
       <c r="Y148" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA148" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="149" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:27" ht="192">
       <c r="A149" s="6" t="s">
         <v>1182</v>
       </c>
@@ -24059,13 +24139,13 @@
         <v>500</v>
       </c>
       <c r="Y149" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA149" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="150" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:27" ht="176">
       <c r="A150" s="9" t="s">
         <v>1190</v>
       </c>
@@ -24125,7 +24205,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="151" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:27" ht="272">
       <c r="A151" s="2" t="s">
         <v>1198</v>
       </c>
@@ -24185,7 +24265,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="152" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:27" ht="160">
       <c r="A152" s="2" t="s">
         <v>1206</v>
       </c>
@@ -24245,7 +24325,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="153" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:27" ht="272">
       <c r="A153" s="2" t="s">
         <v>1214</v>
       </c>
@@ -24305,7 +24385,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="154" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:27" ht="192">
       <c r="A154" s="9" t="s">
         <v>1222</v>
       </c>
@@ -24365,7 +24445,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="155" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:27" ht="144">
       <c r="A155" s="9" t="s">
         <v>1230</v>
       </c>
@@ -24425,7 +24505,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="156" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:27" ht="224">
       <c r="A156" s="2" t="s">
         <v>1238</v>
       </c>
@@ -24487,9 +24567,9 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="157" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:27" ht="176">
       <c r="A157" s="9" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>24</v>
@@ -24549,9 +24629,9 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="158" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:27" ht="176">
       <c r="A158" s="9" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="B158" s="5" t="s">
         <v>24</v>
@@ -24611,9 +24691,9 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="159" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:27" ht="176">
       <c r="A159" s="9" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="B159" s="5" t="s">
         <v>24</v>
@@ -24673,9 +24753,9 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="160" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:27" ht="176">
       <c r="A160" s="9" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>24</v>
@@ -24735,7 +24815,7 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="161" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:27" ht="224">
       <c r="A161" s="2" t="s">
         <v>1276</v>
       </c>
@@ -24795,7 +24875,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="162" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:27" ht="304">
       <c r="A162" s="2" t="s">
         <v>1284</v>
       </c>
@@ -24855,7 +24935,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="163" spans="1:27" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:27" ht="304">
       <c r="A163" s="2" t="s">
         <v>1292</v>
       </c>
@@ -24915,7 +24995,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="164" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:27" ht="272">
       <c r="A164" s="2" t="s">
         <v>1300</v>
       </c>
@@ -24975,7 +25055,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="165" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:27" ht="380">
       <c r="A165" s="9" t="s">
         <v>2689</v>
       </c>
@@ -25035,7 +25115,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="166" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:27" ht="192">
       <c r="A166" s="9" t="s">
         <v>1315</v>
       </c>
@@ -25095,7 +25175,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="167" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:27" ht="192">
       <c r="A167" s="9" t="s">
         <v>1323</v>
       </c>
@@ -25155,7 +25235,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="168" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:27" ht="176">
       <c r="A168" s="9" t="s">
         <v>1332</v>
       </c>
@@ -25215,7 +25295,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="169" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:27" ht="160">
       <c r="A169" s="9" t="s">
         <v>1340</v>
       </c>
@@ -25275,7 +25355,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="170" spans="1:27" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:27" ht="395">
       <c r="A170" s="2" t="s">
         <v>1348</v>
       </c>
@@ -25335,7 +25415,7 @@
         <v>2651</v>
       </c>
     </row>
-    <row r="171" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:27" ht="192">
       <c r="A171" s="9" t="s">
         <v>1357</v>
       </c>
@@ -25395,7 +25475,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="172" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:27" ht="192">
       <c r="A172" s="2" t="s">
         <v>1365</v>
       </c>
@@ -25455,7 +25535,7 @@
         <v>2644</v>
       </c>
     </row>
-    <row r="173" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:27" ht="176">
       <c r="A173" s="2" t="s">
         <v>1373</v>
       </c>
@@ -25515,7 +25595,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="174" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:27" ht="176">
       <c r="A174" s="9" t="s">
         <v>1381</v>
       </c>
@@ -25575,7 +25655,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="175" spans="1:27" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:27" ht="320">
       <c r="A175" s="6" t="s">
         <v>1389</v>
       </c>
@@ -25631,13 +25711,13 @@
         <v>269</v>
       </c>
       <c r="Y175" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA175" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="176" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:27" ht="272">
       <c r="A176" s="2" t="s">
         <v>1397</v>
       </c>
@@ -25697,7 +25777,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="177" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:27" ht="272">
       <c r="A177" s="6" t="s">
         <v>1405</v>
       </c>
@@ -25753,13 +25833,13 @@
         <v>269</v>
       </c>
       <c r="Y177" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA177" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="178" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:27" ht="304">
       <c r="A178" s="2" t="s">
         <v>1413</v>
       </c>
@@ -25819,7 +25899,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="179" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:27" ht="304">
       <c r="A179" s="2" t="s">
         <v>1421</v>
       </c>
@@ -25879,7 +25959,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="180" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:27" ht="272">
       <c r="A180" s="2" t="s">
         <v>1429</v>
       </c>
@@ -25939,7 +26019,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="181" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:27" ht="288">
       <c r="A181" s="2" t="s">
         <v>1437</v>
       </c>
@@ -25999,7 +26079,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="182" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:27" ht="224">
       <c r="A182" s="2" t="s">
         <v>1445</v>
       </c>
@@ -26059,7 +26139,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="183" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:27" ht="160">
       <c r="A183" s="2" t="s">
         <v>1453</v>
       </c>
@@ -26119,7 +26199,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="184" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:27" ht="208">
       <c r="A184" s="2" t="s">
         <v>1462</v>
       </c>
@@ -26179,7 +26259,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="185" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:27" ht="365">
       <c r="A185" s="9" t="s">
         <v>2690</v>
       </c>
@@ -26239,7 +26319,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="186" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:27" ht="160">
       <c r="A186" s="9" t="s">
         <v>1477</v>
       </c>
@@ -26299,7 +26379,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="187" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:27" ht="409.6">
       <c r="A187" s="1" t="s">
         <v>1485</v>
       </c>
@@ -26355,13 +26435,13 @@
         <v>1492</v>
       </c>
       <c r="Y187" s="3" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="AA187" s="10" t="s">
         <v>2622</v>
       </c>
     </row>
-    <row r="188" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:27" ht="208">
       <c r="A188" s="9" t="s">
         <v>2691</v>
       </c>
@@ -26421,7 +26501,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="189" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:27" ht="409.6">
       <c r="A189" s="9" t="s">
         <v>2692</v>
       </c>
@@ -26481,7 +26561,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="190" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:27" ht="380">
       <c r="A190" s="9" t="s">
         <v>2693</v>
       </c>
@@ -26541,7 +26621,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="191" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:27" ht="350">
       <c r="A191" s="9" t="s">
         <v>2694</v>
       </c>
@@ -26601,7 +26681,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="192" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:27" ht="380">
       <c r="A192" s="9" t="s">
         <v>2695</v>
       </c>
@@ -26661,7 +26741,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="193" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:27" ht="192">
       <c r="A193" s="9" t="s">
         <v>2696</v>
       </c>
@@ -26721,7 +26801,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="194" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:27" ht="350">
       <c r="A194" s="9" t="s">
         <v>2697</v>
       </c>
@@ -26781,7 +26861,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="195" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:27" ht="409.6">
       <c r="A195" s="9" t="s">
         <v>2698</v>
       </c>
@@ -26841,7 +26921,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="196" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:27" ht="176">
       <c r="A196" s="9" t="s">
         <v>2699</v>
       </c>
@@ -26901,7 +26981,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="197" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:27" ht="256">
       <c r="A197" s="9" t="s">
         <v>2700</v>
       </c>
@@ -26961,7 +27041,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="198" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:27" ht="409.6">
       <c r="A198" s="9" t="s">
         <v>2701</v>
       </c>
@@ -27021,7 +27101,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="199" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:27" ht="409.6">
       <c r="A199" s="9" t="s">
         <v>2702</v>
       </c>
@@ -27081,7 +27161,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="200" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:27" ht="409.6">
       <c r="A200" s="9" t="s">
         <v>2703</v>
       </c>
@@ -27141,7 +27221,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="201" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:27" ht="409.6">
       <c r="A201" s="9" t="s">
         <v>2704</v>
       </c>
@@ -27201,7 +27281,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="202" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:27" ht="240">
       <c r="A202" s="9" t="s">
         <v>2705</v>
       </c>
@@ -27261,7 +27341,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="203" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:27" ht="208">
       <c r="A203" s="9" t="s">
         <v>2706</v>
       </c>
@@ -27321,7 +27401,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="204" spans="1:27" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:27" ht="395">
       <c r="A204" s="9" t="s">
         <v>2707</v>
       </c>
@@ -27381,7 +27461,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="205" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:27" ht="409.6">
       <c r="A205" s="9" t="s">
         <v>2708</v>
       </c>
@@ -27441,7 +27521,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="206" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:27" ht="380">
       <c r="A206" s="9" t="s">
         <v>2709</v>
       </c>
@@ -27501,7 +27581,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="207" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:27" ht="224">
       <c r="A207" s="9" t="s">
         <v>2710</v>
       </c>
@@ -27561,7 +27641,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="208" spans="1:27" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:27" ht="350">
       <c r="A208" s="9" t="s">
         <v>2711</v>
       </c>
@@ -27621,7 +27701,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="209" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:27" ht="409.6">
       <c r="A209" s="9" t="s">
         <v>2712</v>
       </c>
@@ -27681,7 +27761,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="210" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:27" ht="224">
       <c r="A210" s="9" t="s">
         <v>2713</v>
       </c>
@@ -27741,7 +27821,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="211" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:27" ht="224">
       <c r="A211" s="9" t="s">
         <v>2714</v>
       </c>
@@ -27801,7 +27881,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="212" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:27" ht="224">
       <c r="A212" s="9" t="s">
         <v>2715</v>
       </c>
@@ -27861,7 +27941,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="213" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:27" ht="380">
       <c r="A213" s="9" t="s">
         <v>2716</v>
       </c>
@@ -27921,7 +28001,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="214" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:27" ht="395">
       <c r="A214" s="9" t="s">
         <v>2717</v>
       </c>
@@ -27981,7 +28061,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="215" spans="1:27" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:27" ht="380">
       <c r="A215" s="9" t="s">
         <v>2718</v>
       </c>
@@ -28041,7 +28121,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="216" spans="1:27" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:27" ht="380">
       <c r="A216" s="9" t="s">
         <v>2719</v>
       </c>
@@ -28101,7 +28181,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="217" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:27" ht="395">
       <c r="A217" s="9" t="s">
         <v>2720</v>
       </c>
@@ -28161,7 +28241,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="218" spans="1:27" ht="409.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:27" ht="409" customHeight="1">
       <c r="A218" s="9" t="s">
         <v>2721</v>
       </c>
@@ -28221,7 +28301,7 @@
         <v>2655</v>
       </c>
     </row>
-    <row r="219" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:27" ht="409.6">
       <c r="A219" s="9" t="s">
         <v>2722</v>
       </c>
@@ -28281,9 +28361,9 @@
         <v>2655</v>
       </c>
     </row>
-    <row r="220" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:27" ht="409.6">
       <c r="A220" s="9" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="B220" s="5" t="s">
         <v>24</v>
@@ -28341,9 +28421,9 @@
         <v>2655</v>
       </c>
     </row>
-    <row r="221" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:27" ht="365">
       <c r="A221" s="9" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="B221" s="5" t="s">
         <v>24</v>
@@ -28401,9 +28481,9 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="222" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:27" ht="409.6">
       <c r="A222" s="9" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="B222" s="5" t="s">
         <v>24</v>
@@ -28461,9 +28541,9 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="223" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:27" ht="409.6">
       <c r="A223" s="9" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="B223" s="5" t="s">
         <v>24</v>
@@ -28521,9 +28601,9 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="224" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:27" ht="409.6">
       <c r="A224" s="9" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="B224" s="5" t="s">
         <v>24</v>
@@ -28581,9 +28661,9 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="225" spans="1:27" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:27" ht="380">
       <c r="A225" s="9" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="B225" s="5" t="s">
         <v>24</v>
@@ -28641,9 +28721,9 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="226" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:27" ht="350">
       <c r="A226" s="9" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="B226" s="5" t="s">
         <v>24</v>
@@ -28701,7 +28781,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="227" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:27" ht="350">
       <c r="A227" s="9" t="s">
         <v>2723</v>
       </c>
@@ -28761,7 +28841,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="228" spans="1:27" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:27" ht="395">
       <c r="A228" s="9" t="s">
         <v>2724</v>
       </c>
@@ -28821,7 +28901,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="229" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:27" ht="395">
       <c r="A229" s="9" t="s">
         <v>2725</v>
       </c>
@@ -28881,7 +28961,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="230" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:27" ht="395">
       <c r="A230" s="9" t="s">
         <v>2726</v>
       </c>
@@ -28941,9 +29021,9 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="231" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:27" ht="350">
       <c r="A231" s="9" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="B231" s="5" t="s">
         <v>24</v>
@@ -29001,9 +29081,9 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="232" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:27" ht="350">
       <c r="A232" s="9" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="B232" s="5" t="s">
         <v>24</v>
@@ -29061,7 +29141,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="233" spans="1:27" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:27" ht="380">
       <c r="A233" s="9" t="s">
         <v>2727</v>
       </c>
@@ -29121,7 +29201,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="234" spans="1:27" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:27" ht="380">
       <c r="A234" s="9" t="s">
         <v>2728</v>
       </c>
@@ -29181,7 +29261,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="235" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:27" ht="365">
       <c r="A235" s="9" t="s">
         <v>2729</v>
       </c>
@@ -29241,7 +29321,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="236" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:27" ht="365">
       <c r="A236" s="9" t="s">
         <v>2730</v>
       </c>
@@ -29301,7 +29381,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="237" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:27" ht="176">
       <c r="A237" s="2" t="s">
         <v>1835</v>
       </c>
@@ -29361,7 +29441,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="238" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:27" ht="192">
       <c r="A238" s="2" t="s">
         <v>1843</v>
       </c>
@@ -29421,7 +29501,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="239" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:27" ht="176">
       <c r="A239" s="2" t="s">
         <v>1850</v>
       </c>
@@ -29481,7 +29561,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="240" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:27" ht="192">
       <c r="A240" s="2" t="s">
         <v>1857</v>
       </c>
@@ -29541,9 +29621,9 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="241" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:27" ht="240">
       <c r="A241" s="9" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="B241" s="5" t="s">
         <v>24</v>
@@ -29601,9 +29681,9 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="242" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:27" ht="224">
       <c r="A242" s="9" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="B242" s="5" t="s">
         <v>24</v>
@@ -29661,9 +29741,9 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="243" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:27" ht="224">
       <c r="A243" s="9" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="B243" s="5" t="s">
         <v>24</v>
@@ -29721,9 +29801,9 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="244" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:27" ht="224">
       <c r="A244" s="9" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="B244" s="5" t="s">
         <v>24</v>
@@ -29781,7 +29861,7 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="245" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:27" ht="160">
       <c r="A245" s="2" t="s">
         <v>1891</v>
       </c>
@@ -29843,7 +29923,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="246" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:27" ht="224">
       <c r="A246" s="2" t="s">
         <v>1899</v>
       </c>
@@ -29903,7 +29983,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="247" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:27" ht="160">
       <c r="A247" s="2" t="s">
         <v>1906</v>
       </c>
@@ -29965,7 +30045,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="248" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:27" ht="160">
       <c r="A248" s="2" t="s">
         <v>1913</v>
       </c>
@@ -30027,7 +30107,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="249" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:27" ht="192">
       <c r="A249" s="2" t="s">
         <v>1920</v>
       </c>
@@ -30089,9 +30169,9 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="250" spans="1:27" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:27" ht="320">
       <c r="A250" s="9" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="B250" s="5" t="s">
         <v>60</v>
@@ -30149,7 +30229,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="251" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:27" ht="409.6">
       <c r="A251" s="1" t="s">
         <v>1934</v>
       </c>
@@ -30166,17 +30246,17 @@
         <v>1937</v>
       </c>
       <c r="F251" s="4" t="s">
+        <v>2774</v>
+      </c>
+      <c r="G251" s="4" t="s">
         <v>2775</v>
-      </c>
-      <c r="G251" s="4" t="s">
-        <v>2776</v>
       </c>
       <c r="H251" s="5"/>
       <c r="I251" s="4" t="s">
+        <v>2776</v>
+      </c>
+      <c r="J251" s="4" t="s">
         <v>2777</v>
-      </c>
-      <c r="J251" s="4" t="s">
-        <v>2778</v>
       </c>
       <c r="K251" s="5"/>
       <c r="L251" s="5"/>
@@ -30205,13 +30285,13 @@
         <v>1938</v>
       </c>
       <c r="Y251" s="3" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="AA251" s="10" t="s">
         <v>2657</v>
       </c>
     </row>
-    <row r="252" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:27" ht="409.6">
       <c r="A252" s="1" t="s">
         <v>1934</v>
       </c>
@@ -30228,17 +30308,17 @@
         <v>1941</v>
       </c>
       <c r="F252" s="4" t="s">
+        <v>2779</v>
+      </c>
+      <c r="G252" s="4" t="s">
         <v>2780</v>
-      </c>
-      <c r="G252" s="4" t="s">
-        <v>2781</v>
       </c>
       <c r="H252" s="5"/>
       <c r="I252" s="4" t="s">
+        <v>2781</v>
+      </c>
+      <c r="J252" s="4" t="s">
         <v>2782</v>
-      </c>
-      <c r="J252" s="4" t="s">
-        <v>2783</v>
       </c>
       <c r="K252" s="5"/>
       <c r="L252" s="5"/>
@@ -30267,13 +30347,13 @@
         <v>1938</v>
       </c>
       <c r="Y252" s="3" t="s">
-        <v>2779</v>
+        <v>2778</v>
       </c>
       <c r="AA252" s="10" t="s">
         <v>2657</v>
       </c>
     </row>
-    <row r="253" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:27" ht="256">
       <c r="A253" s="9" t="s">
         <v>2731</v>
       </c>
@@ -30333,7 +30413,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="254" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:27" ht="176">
       <c r="A254" s="6" t="s">
         <v>1949</v>
       </c>
@@ -30389,13 +30469,13 @@
         <v>269</v>
       </c>
       <c r="Y254" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA254" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="255" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:27" ht="304">
       <c r="A255" s="2" t="s">
         <v>1957</v>
       </c>
@@ -30455,7 +30535,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="256" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:27" ht="409.6">
       <c r="A256" s="9" t="s">
         <v>1965</v>
       </c>
@@ -30515,7 +30595,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="257" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:27" ht="304">
       <c r="A257" s="9" t="s">
         <v>1973</v>
       </c>
@@ -30575,7 +30655,7 @@
         <v>2658</v>
       </c>
     </row>
-    <row r="258" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:27" ht="208">
       <c r="A258" s="9" t="s">
         <v>1982</v>
       </c>
@@ -30637,7 +30717,7 @@
         <v>2659</v>
       </c>
     </row>
-    <row r="259" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:27" ht="144">
       <c r="A259" s="9" t="s">
         <v>1991</v>
       </c>
@@ -30697,7 +30777,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="260" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:27" ht="144">
       <c r="A260" s="9" t="s">
         <v>1999</v>
       </c>
@@ -30759,7 +30839,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="261" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:27" ht="160">
       <c r="A261" s="9" t="s">
         <v>2008</v>
       </c>
@@ -30821,9 +30901,9 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="262" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:27" ht="409.6">
       <c r="A262" s="1" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
       <c r="B262" s="5" t="s">
         <v>24</v>
@@ -30838,17 +30918,17 @@
         <v>2019</v>
       </c>
       <c r="F262" s="4" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
       <c r="G262" s="4" t="s">
         <v>2020</v>
       </c>
       <c r="H262" s="5"/>
       <c r="I262" s="4" t="s">
+        <v>2785</v>
+      </c>
+      <c r="J262" s="4" t="s">
         <v>2786</v>
-      </c>
-      <c r="J262" s="4" t="s">
-        <v>2787</v>
       </c>
       <c r="K262" s="5"/>
       <c r="L262" s="5"/>
@@ -30881,7 +30961,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="263" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:27" ht="160">
       <c r="A263" s="9" t="s">
         <v>2021</v>
       </c>
@@ -30943,9 +31023,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="264" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:27" ht="395">
       <c r="A264" s="9" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>24</v>
@@ -31003,9 +31083,9 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="265" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:27" ht="395">
       <c r="A265" s="9" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>24</v>
@@ -31063,7 +31143,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="266" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:27" ht="208">
       <c r="A266" s="9" t="s">
         <v>2042</v>
       </c>
@@ -31125,9 +31205,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="267" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:27" ht="144">
       <c r="A267" s="2" t="s">
-        <v>2789</v>
+        <v>2788</v>
       </c>
       <c r="B267" s="5" t="s">
         <v>24</v>
@@ -31187,7 +31267,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="268" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:27" ht="176">
       <c r="A268" s="6" t="s">
         <v>2674</v>
       </c>
@@ -31243,13 +31323,13 @@
         <v>2066</v>
       </c>
       <c r="Y268" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA268" s="10" t="s">
         <v>2660</v>
       </c>
     </row>
-    <row r="269" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:27" ht="176">
       <c r="A269" s="9" t="s">
         <v>2067</v>
       </c>
@@ -31311,7 +31391,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="270" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:27" ht="208">
       <c r="A270" s="6" t="s">
         <v>2075</v>
       </c>
@@ -31369,13 +31449,13 @@
         <v>269</v>
       </c>
       <c r="Y270" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA270" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="271" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:27" ht="192">
       <c r="A271" s="6" t="s">
         <v>2083</v>
       </c>
@@ -31433,13 +31513,13 @@
         <v>269</v>
       </c>
       <c r="Y271" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA271" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
-    <row r="272" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:27" ht="224">
       <c r="A272" s="9" t="s">
         <v>2091</v>
       </c>
@@ -31501,7 +31581,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="273" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:27" ht="224">
       <c r="A273" s="9" t="s">
         <v>2100</v>
       </c>
@@ -31561,7 +31641,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="274" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:27" ht="176">
       <c r="A274" s="2" t="s">
         <v>2108</v>
       </c>
@@ -31623,7 +31703,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="275" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:27" ht="160">
       <c r="A275" s="2" t="s">
         <v>2116</v>
       </c>
@@ -31685,7 +31765,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="276" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:27" ht="160">
       <c r="A276" s="2" t="s">
         <v>2124</v>
       </c>
@@ -31747,7 +31827,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="277" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:27" ht="208">
       <c r="A277" s="2" t="s">
         <v>2132</v>
       </c>
@@ -31807,7 +31887,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="278" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:27" ht="192">
       <c r="A278" s="9" t="s">
         <v>2140</v>
       </c>
@@ -31869,9 +31949,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="279" spans="1:27" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:27" ht="192">
       <c r="A279" s="1" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
       <c r="B279" s="5" t="s">
         <v>24</v>
@@ -31889,7 +31969,7 @@
         <v>2151</v>
       </c>
       <c r="G279" s="3" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
       <c r="H279" s="5" t="s">
         <v>2014</v>
@@ -31931,7 +32011,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="280" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:27" ht="208">
       <c r="A280" s="2" t="s">
         <v>2154</v>
       </c>
@@ -31993,7 +32073,7 @@
         <v>2661</v>
       </c>
     </row>
-    <row r="281" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:27" ht="409.6">
       <c r="A281" s="2" t="s">
         <v>2163</v>
       </c>
@@ -32053,7 +32133,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="282" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:27" ht="240">
       <c r="A282" s="2" t="s">
         <v>2171</v>
       </c>
@@ -32113,7 +32193,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="283" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:27" ht="176">
       <c r="A283" s="2" t="s">
         <v>2179</v>
       </c>
@@ -32175,7 +32255,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="284" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:27" ht="380">
       <c r="A284" s="9" t="s">
         <v>2187</v>
       </c>
@@ -32235,7 +32315,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="285" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:27" ht="224">
       <c r="A285" s="9" t="s">
         <v>2195</v>
       </c>
@@ -32295,7 +32375,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="286" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:27" ht="192">
       <c r="A286" s="9" t="s">
         <v>2203</v>
       </c>
@@ -32357,7 +32437,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="287" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:27" ht="350">
       <c r="A287" s="6" t="s">
         <v>2211</v>
       </c>
@@ -32419,7 +32499,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="288" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:27" ht="192">
       <c r="A288" s="9" t="s">
         <v>2219</v>
       </c>
@@ -32481,7 +32561,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="289" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:27" ht="192">
       <c r="A289" s="9" t="s">
         <v>2227</v>
       </c>
@@ -32541,7 +32621,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="290" spans="1:27" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:27" ht="350">
       <c r="A290" s="6" t="s">
         <v>2234</v>
       </c>
@@ -32603,7 +32683,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="291" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:27" ht="176">
       <c r="A291" s="6" t="s">
         <v>2241</v>
       </c>
@@ -32661,13 +32741,13 @@
         <v>500</v>
       </c>
       <c r="Y291" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA291" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
-    <row r="292" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:27" ht="395">
       <c r="A292" s="2" t="s">
         <v>2249</v>
       </c>
@@ -32729,7 +32809,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="293" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:27" ht="395">
       <c r="A293" s="2" t="s">
         <v>2259</v>
       </c>
@@ -32791,7 +32871,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="294" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:27" ht="395">
       <c r="A294" s="2" t="s">
         <v>2267</v>
       </c>
@@ -32853,9 +32933,9 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="295" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:27" ht="240">
       <c r="A295" s="1" t="s">
-        <v>2797</v>
+        <v>2796</v>
       </c>
       <c r="B295" s="5" t="s">
         <v>60</v>
@@ -32877,7 +32957,7 @@
       </c>
       <c r="H295" s="5"/>
       <c r="I295" s="4" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="J295" s="5" t="s">
         <v>2280</v>
@@ -32909,15 +32989,15 @@
         <v>35</v>
       </c>
       <c r="Y295" s="13" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="AA295" s="10" t="s">
         <v>2619</v>
       </c>
     </row>
-    <row r="296" spans="1:27" ht="288" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:27" ht="288">
       <c r="A296" s="1" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>24</v>
@@ -32932,17 +33012,17 @@
         <v>2283</v>
       </c>
       <c r="F296" s="4" t="s">
+        <v>2792</v>
+      </c>
+      <c r="G296" s="4" t="s">
         <v>2793</v>
-      </c>
-      <c r="G296" s="4" t="s">
-        <v>2794</v>
       </c>
       <c r="H296" s="5"/>
       <c r="I296" s="4" t="s">
+        <v>2794</v>
+      </c>
+      <c r="J296" s="4" t="s">
         <v>2795</v>
-      </c>
-      <c r="J296" s="4" t="s">
-        <v>2796</v>
       </c>
       <c r="K296" s="5"/>
       <c r="L296" s="5"/>
@@ -32975,7 +33055,7 @@
         <v>2664</v>
       </c>
     </row>
-    <row r="297" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:27" ht="224">
       <c r="A297" s="9" t="s">
         <v>2285</v>
       </c>
@@ -33035,7 +33115,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="298" spans="1:27" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:27" ht="288">
       <c r="A298" s="9" t="s">
         <v>2293</v>
       </c>
@@ -33095,7 +33175,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="299" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:27" ht="224">
       <c r="A299" s="9" t="s">
         <v>2301</v>
       </c>
@@ -33155,7 +33235,7 @@
         <v>2665</v>
       </c>
     </row>
-    <row r="300" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:27" ht="192">
       <c r="A300" s="2" t="s">
         <v>2310</v>
       </c>
@@ -33217,7 +33297,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="301" spans="1:27" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:27" ht="192">
       <c r="A301" s="2" t="s">
         <v>2318</v>
       </c>
@@ -33279,9 +33359,9 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="302" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:27" ht="144">
       <c r="A302" s="2" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="B302" s="5" t="s">
         <v>60</v>
@@ -33341,9 +33421,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="303" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:27" ht="272">
       <c r="A303" s="1" t="s">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="B303" s="5" t="s">
         <v>60</v>
@@ -33365,7 +33445,7 @@
       </c>
       <c r="H303" s="5"/>
       <c r="I303" s="4" t="s">
-        <v>2801</v>
+        <v>2800</v>
       </c>
       <c r="J303" s="5" t="s">
         <v>2339</v>
@@ -33397,13 +33477,13 @@
         <v>35</v>
       </c>
       <c r="Y303" s="13" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="AA303" s="10" t="s">
         <v>2619</v>
       </c>
     </row>
-    <row r="304" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:27" ht="409.6">
       <c r="A304" s="9" t="s">
         <v>2732</v>
       </c>
@@ -33463,7 +33543,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="305" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:27" ht="409.6">
       <c r="A305" s="9" t="s">
         <v>2733</v>
       </c>
@@ -33523,7 +33603,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="306" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:27" ht="409.6">
       <c r="A306" s="6" t="s">
         <v>2676</v>
       </c>
@@ -33579,13 +33659,13 @@
         <v>2360</v>
       </c>
       <c r="Y306" s="3" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="AA306" s="10" t="s">
         <v>2667</v>
       </c>
     </row>
-    <row r="307" spans="1:27" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:27" ht="240">
       <c r="A307" s="9" t="s">
         <v>2361</v>
       </c>
@@ -33647,9 +33727,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="308" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:27" ht="409.6">
       <c r="A308" s="9" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="B308" s="5" t="s">
         <v>24</v>
@@ -33709,7 +33789,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="309" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:27" ht="409.6">
       <c r="A309" s="9" t="s">
         <v>2734</v>
       </c>
@@ -33771,7 +33851,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="310" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:27" ht="176">
       <c r="A310" s="9" t="s">
         <v>2383</v>
       </c>
@@ -33833,7 +33913,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="311" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:27" ht="144">
       <c r="A311" s="9" t="s">
         <v>2391</v>
       </c>
@@ -33895,9 +33975,9 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="312" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:27" ht="409.6">
       <c r="A312" s="1" t="s">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="B312" s="3" t="s">
         <v>2618</v>
@@ -33951,15 +34031,15 @@
         <v>1938</v>
       </c>
       <c r="Y312" s="3" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="AA312" s="10" t="s">
         <v>2657</v>
       </c>
     </row>
-    <row r="313" spans="1:27" ht="144" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:27" ht="144">
       <c r="A313" s="2" t="s">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="B313" s="5" t="s">
         <v>24</v>
@@ -34019,7 +34099,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="314" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:27" ht="224">
       <c r="A314" s="2" t="s">
         <v>2413</v>
       </c>
@@ -34079,7 +34159,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="315" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:27" ht="409.6">
       <c r="A315" s="2" t="s">
         <v>2421</v>
       </c>
@@ -34139,7 +34219,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="316" spans="1:27" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:27" ht="224">
       <c r="A316" s="2" t="s">
         <v>2430</v>
       </c>
@@ -34199,7 +34279,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="317" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:27" ht="240">
       <c r="A317" s="9" t="s">
         <v>2438</v>
       </c>
@@ -34259,7 +34339,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="318" spans="1:27" ht="216" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:27" ht="240">
       <c r="A318" s="9" t="s">
         <v>2446</v>
       </c>
@@ -34319,7 +34399,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="319" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:27" ht="380">
       <c r="A319" s="9" t="s">
         <v>2735</v>
       </c>
@@ -34379,7 +34459,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="320" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:27" ht="409.6">
       <c r="A320" s="2" t="s">
         <v>2461</v>
       </c>
@@ -34439,7 +34519,7 @@
         <v>2669</v>
       </c>
     </row>
-    <row r="321" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:27" ht="409.6">
       <c r="A321" s="9" t="s">
         <v>2470</v>
       </c>
@@ -34499,7 +34579,7 @@
         <v>2657</v>
       </c>
     </row>
-    <row r="322" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:27" ht="409.6">
       <c r="A322" s="9" t="s">
         <v>2479</v>
       </c>
@@ -34559,7 +34639,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="323" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:27" ht="409.6">
       <c r="A323" s="2" t="s">
         <v>2488</v>
       </c>
@@ -34619,9 +34699,9 @@
         <v>2671</v>
       </c>
     </row>
-    <row r="324" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:27" ht="409.6">
       <c r="A324" s="1" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="B324" s="5" t="s">
         <v>24</v>
@@ -34636,17 +34716,17 @@
         <v>2499</v>
       </c>
       <c r="F324" s="4" t="s">
+        <v>2804</v>
+      </c>
+      <c r="G324" s="4" t="s">
         <v>2805</v>
-      </c>
-      <c r="G324" s="4" t="s">
-        <v>2806</v>
       </c>
       <c r="H324" s="5"/>
       <c r="I324" s="4" t="s">
+        <v>2806</v>
+      </c>
+      <c r="J324" s="4" t="s">
         <v>2807</v>
-      </c>
-      <c r="J324" s="4" t="s">
-        <v>2808</v>
       </c>
       <c r="K324" s="5"/>
       <c r="L324" s="5"/>
@@ -34679,7 +34759,7 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="325" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:27" ht="409.6">
       <c r="A325" s="1" t="s">
         <v>2501</v>
       </c>
@@ -34696,17 +34776,17 @@
         <v>2504</v>
       </c>
       <c r="F325" s="4" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="G325" s="5" t="s">
         <v>2505</v>
       </c>
       <c r="H325" s="5"/>
       <c r="I325" s="4" t="s">
+        <v>2810</v>
+      </c>
+      <c r="J325" s="4" t="s">
         <v>2811</v>
-      </c>
-      <c r="J325" s="4" t="s">
-        <v>2812</v>
       </c>
       <c r="K325" s="5"/>
       <c r="L325" s="5"/>
@@ -34739,7 +34819,7 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="326" spans="1:27" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:27" ht="176">
       <c r="A326" s="6" t="s">
         <v>2675</v>
       </c>
@@ -34795,13 +34875,13 @@
         <v>2066</v>
       </c>
       <c r="Y326" s="3" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="AA326" s="10" t="s">
         <v>2660</v>
       </c>
     </row>
-    <row r="327" spans="1:27" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:27" ht="365">
       <c r="A327" s="2" t="s">
         <v>2513</v>
       </c>
@@ -34861,7 +34941,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="328" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:27" ht="288">
       <c r="A328" s="2" t="s">
         <v>2522</v>
       </c>
@@ -34921,7 +35001,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="329" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:27" ht="395">
       <c r="A329" s="2" t="s">
         <v>2530</v>
       </c>
@@ -34981,7 +35061,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="330" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:27" ht="409.6">
       <c r="A330" s="2" t="s">
         <v>2538</v>
       </c>
@@ -35041,7 +35121,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="331" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:27" ht="395">
       <c r="A331" s="2" t="s">
         <v>2545</v>
       </c>
@@ -35101,7 +35181,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="332" spans="1:27" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:27" ht="272">
       <c r="A332" s="9" t="s">
         <v>2552</v>
       </c>
@@ -35161,7 +35241,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="333" spans="1:27" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:27" ht="380">
       <c r="A333" s="9" t="s">
         <v>2736</v>
       </c>
@@ -35221,7 +35301,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="334" spans="1:27" ht="360" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:27" ht="365">
       <c r="A334" s="9" t="s">
         <v>2737</v>
       </c>
@@ -35281,7 +35361,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="335" spans="1:27" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:27" ht="380">
       <c r="A335" s="9" t="s">
         <v>2738</v>
       </c>
@@ -35341,7 +35421,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="336" spans="1:27" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:27" ht="380">
       <c r="A336" s="9" t="s">
         <v>2739</v>
       </c>
@@ -35401,7 +35481,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="337" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:27" ht="409.6">
       <c r="A337" s="9" t="s">
         <v>2588</v>
       </c>
@@ -35461,7 +35541,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="338" spans="1:27" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:27" ht="409.6">
       <c r="A338" s="2" t="s">
         <v>2596</v>
       </c>
@@ -35521,7 +35601,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="339" spans="1:27" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:27" ht="240">
       <c r="A339" s="2" t="s">
         <v>2604</v>
       </c>

</xml_diff>